<commit_message>
Task Graph for V0CE
</commit_message>
<xml_diff>
--- a/TaskgraphsEdgeDetect/hwsw-partitioning/TaskGraph-Attributes.xlsx
+++ b/TaskgraphsEdgeDetect/hwsw-partitioning/TaskGraph-Attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Dev\Experiments\TaskgraphsEdgeDetect\hwsw-partitioning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD33E6F0-8CD8-4DBF-8FDB-74976E8DD6C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D5B146-117D-4D60-9DDE-A810A64D2DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V0" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="43">
   <si>
     <t>latency</t>
   </si>
@@ -130,18 +130,6 @@
   </si>
   <si>
     <t>RoundtripCopyTime (us)</t>
-  </si>
-  <si>
-    <t>m-oneway</t>
-  </si>
-  <si>
-    <t>b-oneway</t>
-  </si>
-  <si>
-    <t>m-roundtrip</t>
-  </si>
-  <si>
-    <t>b-roundtrip</t>
   </si>
   <si>
     <t>set_filter_vertical</t>
@@ -426,16 +414,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -472,51 +458,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -529,7 +474,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -554,7 +499,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -563,6 +508,48 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,6 +611,61 @@
         <a:xfrm>
           <a:off x="11725275" y="76200"/>
           <a:ext cx="4039613" cy="6572250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD500D6C-D3CB-DE92-D4DB-D446EFD8F662}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11896725" y="47625"/>
+          <a:ext cx="4686300" cy="6200775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -900,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,48 +960,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="34"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="61"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="25" t="s">
+      <c r="A2" s="63"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="25" t="s">
+      <c r="E2" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="24" t="s">
         <v>5</v>
       </c>
     </row>
@@ -970,7 +1012,7 @@
       <c r="B3" s="2">
         <v>143601</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="9">
         <f>$D3 * 1000000</f>
         <v>2871.1593500000004</v>
       </c>
@@ -983,16 +1025,16 @@
       <c r="F3" s="2">
         <v>273.97260273972603</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="12">
         <v>1.3271672504378201E-2</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="12">
         <v>5.0492556917688197E-2</v>
       </c>
-      <c r="I3" s="14">
-        <v>0</v>
-      </c>
-      <c r="J3" s="15">
+      <c r="I3" s="12">
+        <v>0</v>
+      </c>
+      <c r="J3" s="13">
         <v>5.5555555555555497E-3</v>
       </c>
     </row>
@@ -1000,32 +1042,32 @@
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="41">
+      <c r="B4">
         <v>14467</v>
       </c>
-      <c r="C4" s="42">
+      <c r="C4" s="10">
         <f t="shared" ref="C4:C9" si="0">$D4 * 1000000</f>
         <v>8546.0698500000017</v>
       </c>
-      <c r="D4" s="41">
+      <c r="D4">
         <v>8.5460698500000008E-3</v>
       </c>
-      <c r="E4" s="41">
+      <c r="E4">
         <v>2341389</v>
       </c>
-      <c r="F4" s="41">
+      <c r="F4">
         <v>273.97260273972603</v>
       </c>
-      <c r="G4" s="43">
+      <c r="G4" s="31">
         <v>2.6514156450671299E-2</v>
       </c>
-      <c r="H4" s="43">
+      <c r="H4" s="31">
         <v>0.133413601868067</v>
       </c>
-      <c r="I4" s="43">
-        <v>0</v>
-      </c>
-      <c r="J4" s="16">
+      <c r="I4" s="31">
+        <v>0</v>
+      </c>
+      <c r="J4" s="14">
         <v>1.0714285714285701E-2</v>
       </c>
     </row>
@@ -1033,32 +1075,32 @@
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="41">
+      <c r="B5">
         <v>245034</v>
       </c>
-      <c r="C5" s="42">
+      <c r="C5" s="10">
         <f t="shared" si="0"/>
         <v>1914.1877500000001</v>
       </c>
-      <c r="D5" s="41">
+      <c r="D5">
         <v>1.91418775E-3</v>
       </c>
-      <c r="E5" s="41">
+      <c r="E5">
         <v>524435</v>
       </c>
-      <c r="F5" s="41">
+      <c r="F5">
         <v>273.97260273972603</v>
       </c>
-      <c r="G5" s="43">
+      <c r="G5" s="31">
         <v>7.8309252772912993E-2</v>
       </c>
-      <c r="H5" s="43">
+      <c r="H5" s="31">
         <v>2.1555750145942701E-2</v>
       </c>
-      <c r="I5" s="43">
-        <v>0</v>
-      </c>
-      <c r="J5" s="16">
+      <c r="I5" s="31">
+        <v>0</v>
+      </c>
+      <c r="J5" s="14">
         <v>0</v>
       </c>
     </row>
@@ -1066,155 +1108,155 @@
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="41">
-        <v>0</v>
-      </c>
-      <c r="C6" s="42">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="10">
         <f t="shared" si="0"/>
         <v>0.2555</v>
       </c>
-      <c r="D6" s="44">
+      <c r="D6" s="32">
         <v>2.5549999999999998E-7</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6">
         <v>70</v>
       </c>
-      <c r="F6" s="41">
+      <c r="F6">
         <v>273.97260273972603</v>
       </c>
-      <c r="G6" s="43">
+      <c r="G6" s="31">
         <v>3.3785755983654401E-3</v>
       </c>
-      <c r="H6" s="43">
+      <c r="H6" s="31">
         <v>1.0402072387624001E-2</v>
       </c>
-      <c r="I6" s="43">
-        <v>0</v>
-      </c>
-      <c r="J6" s="16">
+      <c r="I6" s="31">
+        <v>0</v>
+      </c>
+      <c r="J6" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="41">
-        <v>0</v>
-      </c>
-      <c r="C7" s="42">
+        <v>31</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="10">
         <f t="shared" si="0"/>
         <v>0.2555</v>
       </c>
-      <c r="D7" s="44">
+      <c r="D7" s="32">
         <v>2.5549999999999998E-7</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7">
         <v>70</v>
       </c>
-      <c r="F7" s="41">
+      <c r="F7">
         <v>273.97260273972603</v>
       </c>
-      <c r="G7" s="43">
+      <c r="G7" s="31">
         <v>3.3785755983654401E-3</v>
       </c>
-      <c r="H7" s="43">
+      <c r="H7" s="31">
         <v>1.0402072387624001E-2</v>
       </c>
-      <c r="I7" s="43">
-        <v>0</v>
-      </c>
-      <c r="J7" s="16">
+      <c r="I7" s="31">
+        <v>0</v>
+      </c>
+      <c r="J7" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="6">
-        <v>0</v>
-      </c>
-      <c r="C8" s="22">
+      <c r="A8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+      <c r="C8" s="20">
         <f t="shared" si="0"/>
         <v>0.2555</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>2.5549999999999998E-7</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>70</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>273.97260273972603</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="15">
         <v>3.3785755983654401E-3</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="15">
         <v>1.0402072387624001E-2</v>
       </c>
-      <c r="I8" s="17">
-        <v>0</v>
-      </c>
-      <c r="J8" s="18">
+      <c r="I8" s="15">
+        <v>0</v>
+      </c>
+      <c r="J8" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="8">
         <v>435372</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="11">
         <f t="shared" si="0"/>
         <v>534535.19634999998</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="8">
         <v>0.53453519635000002</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="8">
         <v>146447999</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="8">
         <v>273.97260273972603</v>
       </c>
-      <c r="G9" s="45">
+      <c r="G9" s="33">
         <v>0.11206217162872099</v>
       </c>
-      <c r="H9" s="45">
+      <c r="H9" s="33">
         <v>0.19555239346176201</v>
       </c>
-      <c r="I9" s="45">
-        <v>0</v>
-      </c>
-      <c r="J9" s="46">
+      <c r="I9" s="33">
+        <v>0</v>
+      </c>
+      <c r="J9" s="34">
         <v>1.6269841269841202E-2</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="29" t="s">
+      <c r="E12" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="H12" s="51"/>
-      <c r="I12" s="48"/>
+      <c r="G12" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="58"/>
+      <c r="I12" s="59"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1226,21 +1268,21 @@
       <c r="C13" s="2">
         <v>4</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="9">
         <f>$B13*$C13*$I$13 + $I$14</f>
         <v>4562.1665434388442</v>
       </c>
-      <c r="E13" s="30">
+      <c r="E13" s="28">
         <f>$B13*$C13*$I$15 + $I$16</f>
         <v>6671.5308280954259</v>
       </c>
-      <c r="G13" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" s="52" t="s">
-        <v>41</v>
-      </c>
-      <c r="I13" s="4">
+      <c r="G13" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="68">
         <v>1.4582852584745199E-3</v>
       </c>
     </row>
@@ -1254,19 +1296,19 @@
       <c r="C14">
         <v>4</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="10">
         <f>$B14*$C14*$I$13 + $I$14</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="E14" s="31">
+      <c r="E14" s="29">
         <f>$B14*$C14*$I$15 + $I$16</f>
         <v>2207.799534354021</v>
       </c>
-      <c r="G14" s="50"/>
-      <c r="H14" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="I14" s="8">
+      <c r="G14" s="56"/>
+      <c r="H14" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="69">
         <v>-25.202226131690999</v>
       </c>
     </row>
@@ -1280,21 +1322,21 @@
       <c r="C15">
         <v>4</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="10">
         <f>$B15*$C15*$I$13 + $I$14</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="E15" s="31">
+      <c r="E15" s="29">
         <f>$B15*$C15*$I$15 + $I$16</f>
         <v>2207.799534354021</v>
       </c>
-      <c r="G15" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="H15" s="52" t="s">
-        <v>41</v>
-      </c>
-      <c r="I15" s="4">
+      <c r="G15" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15" s="70">
         <v>2.1284729450900099E-3</v>
       </c>
     </row>
@@ -1308,438 +1350,438 @@
       <c r="C16">
         <v>4</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="10">
         <f>$B16*$C16*$I$13 + $I$14</f>
         <v>-25.149727862385916</v>
       </c>
-      <c r="E16" s="31">
+      <c r="E16" s="29">
         <f>$B16*$C16*$I$15 + $I$16</f>
         <v>-23.989487490657858</v>
       </c>
-      <c r="G16" s="50"/>
-      <c r="H16" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="I16" s="8">
+      <c r="G16" s="56"/>
+      <c r="H16" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="I16" s="69">
         <v>-24.066112516681098</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <v>262144</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>4</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="20">
         <f>$B17*$C17*$I$13 + $I$14</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="E17" s="32">
+      <c r="E17" s="30">
         <f>$B17*$C17*$I$15 + $I$16</f>
         <v>2207.799534354021</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="59"/>
-      <c r="B20" s="64" t="s">
+      <c r="A20" s="42"/>
+      <c r="B20" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="57" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="57" t="s">
+      <c r="C20" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="57" t="s">
+      <c r="G20" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="I20" s="57" t="s">
-        <v>36</v>
-      </c>
-      <c r="J20" s="57" t="s">
+      <c r="H20" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="J20" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="K20" s="41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="48">
+        <v>0</v>
+      </c>
+      <c r="C21" s="51">
+        <f>D14</f>
+        <v>1503.9206970584871</v>
+      </c>
+      <c r="D21" s="51">
+        <f>D14</f>
+        <v>1503.9206970584871</v>
+      </c>
+      <c r="E21" s="49">
+        <v>0</v>
+      </c>
+      <c r="F21" s="49">
+        <v>0</v>
+      </c>
+      <c r="G21" s="49">
+        <v>0</v>
+      </c>
+      <c r="H21" s="49">
+        <v>0</v>
+      </c>
+      <c r="I21" s="49">
+        <v>0</v>
+      </c>
+      <c r="J21" s="49">
+        <v>0</v>
+      </c>
+      <c r="K21" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="35">
+        <v>0</v>
+      </c>
+      <c r="C22" s="43">
+        <v>0</v>
+      </c>
+      <c r="D22" s="52">
+        <f>D17</f>
+        <v>1503.9206970584871</v>
+      </c>
+      <c r="E22" s="52">
+        <f>D17</f>
+        <v>1503.9206970584871</v>
+      </c>
+      <c r="F22" s="52">
+        <f>D17</f>
+        <v>1503.9206970584871</v>
+      </c>
+      <c r="G22" s="43">
+        <v>0</v>
+      </c>
+      <c r="H22" s="43">
+        <v>0</v>
+      </c>
+      <c r="I22" s="43">
+        <v>0</v>
+      </c>
+      <c r="J22" s="43">
+        <v>0</v>
+      </c>
+      <c r="K22" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="35">
+        <v>0</v>
+      </c>
+      <c r="C23" s="43">
+        <v>0</v>
+      </c>
+      <c r="D23" s="43">
+        <v>0</v>
+      </c>
+      <c r="E23" s="43">
+        <v>0</v>
+      </c>
+      <c r="F23" s="52">
+        <f>D14</f>
+        <v>1503.9206970584871</v>
+      </c>
+      <c r="G23" s="43">
+        <v>0</v>
+      </c>
+      <c r="H23" s="43">
+        <v>0</v>
+      </c>
+      <c r="I23" s="43">
+        <v>0</v>
+      </c>
+      <c r="J23" s="43">
+        <v>0</v>
+      </c>
+      <c r="K23" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="K20" s="58" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="54" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="65">
-        <v>0</v>
-      </c>
-      <c r="C21" s="68">
-        <f>D14</f>
-        <v>1503.9206970584871</v>
-      </c>
-      <c r="D21" s="68">
-        <f>D14</f>
-        <v>1503.9206970584871</v>
-      </c>
-      <c r="E21" s="66">
-        <v>0</v>
-      </c>
-      <c r="F21" s="66">
-        <v>0</v>
-      </c>
-      <c r="G21" s="66">
-        <v>0</v>
-      </c>
-      <c r="H21" s="66">
-        <v>0</v>
-      </c>
-      <c r="I21" s="66">
-        <v>0</v>
-      </c>
-      <c r="J21" s="66">
-        <v>0</v>
-      </c>
-      <c r="K21" s="67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="55" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="52">
-        <v>0</v>
-      </c>
-      <c r="C22" s="60">
-        <v>0</v>
-      </c>
-      <c r="D22" s="69">
+      <c r="B24" s="35">
+        <v>0</v>
+      </c>
+      <c r="C24" s="43">
+        <v>0</v>
+      </c>
+      <c r="D24" s="43">
+        <v>0</v>
+      </c>
+      <c r="E24" s="43">
+        <v>0</v>
+      </c>
+      <c r="F24" s="52">
+        <f>D15</f>
+        <v>1503.9206970584871</v>
+      </c>
+      <c r="G24" s="43">
+        <v>0</v>
+      </c>
+      <c r="H24" s="43">
+        <v>0</v>
+      </c>
+      <c r="I24" s="43">
+        <v>0</v>
+      </c>
+      <c r="J24" s="43">
+        <v>0</v>
+      </c>
+      <c r="K24" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="35">
+        <v>0</v>
+      </c>
+      <c r="C25" s="43">
+        <v>0</v>
+      </c>
+      <c r="D25" s="43">
+        <v>0</v>
+      </c>
+      <c r="E25" s="43">
+        <v>0</v>
+      </c>
+      <c r="F25" s="43">
+        <v>0</v>
+      </c>
+      <c r="G25" s="43">
+        <v>0</v>
+      </c>
+      <c r="H25" s="43">
+        <v>0</v>
+      </c>
+      <c r="I25" s="43">
+        <v>0</v>
+      </c>
+      <c r="J25" s="43">
+        <v>0</v>
+      </c>
+      <c r="K25" s="53">
         <f>D17</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="E22" s="69">
-        <f>D17</f>
-        <v>1503.9206970584871</v>
-      </c>
-      <c r="F22" s="69">
-        <f>D17</f>
-        <v>1503.9206970584871</v>
-      </c>
-      <c r="G22" s="60">
-        <v>0</v>
-      </c>
-      <c r="H22" s="60">
-        <v>0</v>
-      </c>
-      <c r="I22" s="60">
-        <v>0</v>
-      </c>
-      <c r="J22" s="60">
-        <v>0</v>
-      </c>
-      <c r="K22" s="61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="52">
-        <v>0</v>
-      </c>
-      <c r="C23" s="60">
-        <v>0</v>
-      </c>
-      <c r="D23" s="60">
-        <v>0</v>
-      </c>
-      <c r="E23" s="60">
-        <v>0</v>
-      </c>
-      <c r="F23" s="69">
-        <f>D14</f>
-        <v>1503.9206970584871</v>
-      </c>
-      <c r="G23" s="60">
-        <v>0</v>
-      </c>
-      <c r="H23" s="60">
-        <v>0</v>
-      </c>
-      <c r="I23" s="60">
-        <v>0</v>
-      </c>
-      <c r="J23" s="60">
-        <v>0</v>
-      </c>
-      <c r="K23" s="61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="55" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="52">
-        <v>0</v>
-      </c>
-      <c r="C24" s="60">
-        <v>0</v>
-      </c>
-      <c r="D24" s="60">
-        <v>0</v>
-      </c>
-      <c r="E24" s="60">
-        <v>0</v>
-      </c>
-      <c r="F24" s="69">
-        <f>D15</f>
-        <v>1503.9206970584871</v>
-      </c>
-      <c r="G24" s="60">
-        <v>0</v>
-      </c>
-      <c r="H24" s="60">
-        <v>0</v>
-      </c>
-      <c r="I24" s="60">
-        <v>0</v>
-      </c>
-      <c r="J24" s="60">
-        <v>0</v>
-      </c>
-      <c r="K24" s="61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="52">
-        <v>0</v>
-      </c>
-      <c r="C25" s="60">
-        <v>0</v>
-      </c>
-      <c r="D25" s="60">
-        <v>0</v>
-      </c>
-      <c r="E25" s="60">
-        <v>0</v>
-      </c>
-      <c r="F25" s="60">
-        <v>0</v>
-      </c>
-      <c r="G25" s="60">
-        <v>0</v>
-      </c>
-      <c r="H25" s="60">
-        <v>0</v>
-      </c>
-      <c r="I25" s="60">
-        <v>0</v>
-      </c>
-      <c r="J25" s="60">
-        <v>0</v>
-      </c>
-      <c r="K25" s="70">
-        <f>D17</f>
-        <v>1503.9206970584871</v>
-      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="55" t="s">
+      <c r="A26" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="52">
-        <v>0</v>
-      </c>
-      <c r="C26" s="69">
+      <c r="B26" s="35">
+        <v>0</v>
+      </c>
+      <c r="C26" s="52">
         <f>D16</f>
         <v>-25.149727862385916</v>
       </c>
-      <c r="D26" s="60">
-        <v>0</v>
-      </c>
-      <c r="E26" s="60">
-        <v>0</v>
-      </c>
-      <c r="F26" s="60">
-        <v>0</v>
-      </c>
-      <c r="G26" s="60">
-        <v>0</v>
-      </c>
-      <c r="H26" s="69">
+      <c r="D26" s="43">
+        <v>0</v>
+      </c>
+      <c r="E26" s="43">
+        <v>0</v>
+      </c>
+      <c r="F26" s="43">
+        <v>0</v>
+      </c>
+      <c r="G26" s="43">
+        <v>0</v>
+      </c>
+      <c r="H26" s="52">
         <f>D16</f>
         <v>-25.149727862385916</v>
       </c>
-      <c r="I26" s="60">
-        <v>0</v>
-      </c>
-      <c r="J26" s="60">
-        <v>0</v>
-      </c>
-      <c r="K26" s="61">
+      <c r="I26" s="43">
+        <v>0</v>
+      </c>
+      <c r="J26" s="43">
+        <v>0</v>
+      </c>
+      <c r="K26" s="44">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="52">
-        <v>0</v>
-      </c>
-      <c r="C27" s="60">
-        <v>0</v>
-      </c>
-      <c r="D27" s="69">
+      <c r="A27" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="35">
+        <v>0</v>
+      </c>
+      <c r="C27" s="43">
+        <v>0</v>
+      </c>
+      <c r="D27" s="52">
         <f>D16</f>
         <v>-25.149727862385916</v>
       </c>
-      <c r="E27" s="60">
-        <v>0</v>
-      </c>
-      <c r="F27" s="60">
-        <v>0</v>
-      </c>
-      <c r="G27" s="60">
-        <v>0</v>
-      </c>
-      <c r="H27" s="60">
-        <v>0</v>
-      </c>
-      <c r="I27" s="69">
+      <c r="E27" s="43">
+        <v>0</v>
+      </c>
+      <c r="F27" s="43">
+        <v>0</v>
+      </c>
+      <c r="G27" s="43">
+        <v>0</v>
+      </c>
+      <c r="H27" s="43">
+        <v>0</v>
+      </c>
+      <c r="I27" s="52">
         <f>D16</f>
         <v>-25.149727862385916</v>
       </c>
-      <c r="J27" s="60">
-        <v>0</v>
-      </c>
-      <c r="K27" s="61">
+      <c r="J27" s="43">
+        <v>0</v>
+      </c>
+      <c r="K27" s="44">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="55" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="52">
-        <v>0</v>
-      </c>
-      <c r="C28" s="60">
-        <v>0</v>
-      </c>
-      <c r="D28" s="60">
-        <v>0</v>
-      </c>
-      <c r="E28" s="69">
+      <c r="A28" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="35">
+        <v>0</v>
+      </c>
+      <c r="C28" s="43">
+        <v>0</v>
+      </c>
+      <c r="D28" s="43">
+        <v>0</v>
+      </c>
+      <c r="E28" s="52">
         <f>D16</f>
         <v>-25.149727862385916</v>
       </c>
-      <c r="F28" s="60">
-        <v>0</v>
-      </c>
-      <c r="G28" s="60">
-        <v>0</v>
-      </c>
-      <c r="H28" s="60">
-        <v>0</v>
-      </c>
-      <c r="I28" s="60">
-        <v>0</v>
-      </c>
-      <c r="J28" s="60">
-        <v>0</v>
-      </c>
-      <c r="K28" s="61">
+      <c r="F28" s="43">
+        <v>0</v>
+      </c>
+      <c r="G28" s="43">
+        <v>0</v>
+      </c>
+      <c r="H28" s="43">
+        <v>0</v>
+      </c>
+      <c r="I28" s="43">
+        <v>0</v>
+      </c>
+      <c r="J28" s="43">
+        <v>0</v>
+      </c>
+      <c r="K28" s="44">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="55" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" s="71">
+      <c r="A29" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="54">
         <f>D13+D14</f>
         <v>6066.0872404973315</v>
       </c>
-      <c r="C29" s="69">
+      <c r="C29" s="52">
         <f>D17</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="D29" s="60">
-        <v>0</v>
-      </c>
-      <c r="E29" s="69">
+      <c r="D29" s="43">
+        <v>0</v>
+      </c>
+      <c r="E29" s="52">
         <f>D15</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="F29" s="60">
-        <v>0</v>
-      </c>
-      <c r="G29" s="69">
+      <c r="F29" s="43">
+        <v>0</v>
+      </c>
+      <c r="G29" s="52">
         <f>D16</f>
         <v>-25.149727862385916</v>
       </c>
-      <c r="H29" s="60">
-        <v>0</v>
-      </c>
-      <c r="I29" s="60">
-        <v>0</v>
-      </c>
-      <c r="J29" s="60">
-        <v>0</v>
-      </c>
-      <c r="K29" s="61">
+      <c r="H29" s="43">
+        <v>0</v>
+      </c>
+      <c r="I29" s="43">
+        <v>0</v>
+      </c>
+      <c r="J29" s="43">
+        <v>0</v>
+      </c>
+      <c r="K29" s="44">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="56" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="53">
-        <v>0</v>
-      </c>
-      <c r="C30" s="62">
-        <v>0</v>
-      </c>
-      <c r="D30" s="62">
-        <v>0</v>
-      </c>
-      <c r="E30" s="62">
-        <v>0</v>
-      </c>
-      <c r="F30" s="62">
-        <v>0</v>
-      </c>
-      <c r="G30" s="62">
-        <v>0</v>
-      </c>
-      <c r="H30" s="62">
-        <v>0</v>
-      </c>
-      <c r="I30" s="62">
-        <v>0</v>
-      </c>
-      <c r="J30" s="62">
-        <v>0</v>
-      </c>
-      <c r="K30" s="63">
+      <c r="A30" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="36">
+        <v>0</v>
+      </c>
+      <c r="C30" s="45">
+        <v>0</v>
+      </c>
+      <c r="D30" s="45">
+        <v>0</v>
+      </c>
+      <c r="E30" s="45">
+        <v>0</v>
+      </c>
+      <c r="F30" s="45">
+        <v>0</v>
+      </c>
+      <c r="G30" s="45">
+        <v>0</v>
+      </c>
+      <c r="H30" s="45">
+        <v>0</v>
+      </c>
+      <c r="I30" s="45">
+        <v>0</v>
+      </c>
+      <c r="J30" s="45">
+        <v>0</v>
+      </c>
+      <c r="K30" s="46">
         <v>0</v>
       </c>
     </row>
@@ -1761,10 +1803,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F280CF7-3598-485E-A72B-033C2161085F}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1773,55 +1815,56 @@
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="6" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="34"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="61"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="25" t="s">
+      <c r="A2" s="63"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="25" t="s">
+      <c r="E2" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="24" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1829,31 +1872,31 @@
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="19" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1861,32 +1904,32 @@
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="41">
+      <c r="B4">
         <v>149827</v>
       </c>
-      <c r="C4" s="42">
+      <c r="C4" s="10">
         <f>$D4 * 1000000</f>
         <v>2871.1593500000004</v>
       </c>
-      <c r="D4" s="41">
+      <c r="D4">
         <v>2.8711593500000002E-3</v>
       </c>
-      <c r="E4" s="41">
+      <c r="E4">
         <v>786619</v>
       </c>
-      <c r="F4" s="41">
+      <c r="F4">
         <v>273.97260273972603</v>
       </c>
-      <c r="G4" s="43">
+      <c r="G4" s="31">
         <v>1.3271672504378201E-2</v>
       </c>
-      <c r="H4" s="43">
+      <c r="H4" s="31">
         <v>5.0492556917688197E-2</v>
       </c>
-      <c r="I4" s="43">
-        <v>0</v>
-      </c>
-      <c r="J4" s="16">
+      <c r="I4" s="31">
+        <v>0</v>
+      </c>
+      <c r="J4" s="14">
         <v>5.5555555555555497E-3</v>
       </c>
     </row>
@@ -1894,32 +1937,32 @@
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="41">
+      <c r="B5">
         <v>17706</v>
       </c>
-      <c r="C5" s="42">
+      <c r="C5" s="10">
         <f>$D5 * 1000000</f>
         <v>8544.8069500000001</v>
       </c>
-      <c r="D5" s="41">
+      <c r="D5">
         <v>8.5448069500000008E-3</v>
       </c>
-      <c r="E5" s="41">
+      <c r="E5">
         <v>2341043</v>
       </c>
-      <c r="F5" s="41">
+      <c r="F5">
         <v>273.97260273972603</v>
       </c>
-      <c r="G5" s="43">
+      <c r="G5" s="31">
         <v>3.3986427320490298E-3</v>
       </c>
-      <c r="H5" s="43">
+      <c r="H5" s="31">
         <v>1.04057209573847E-2</v>
       </c>
-      <c r="I5" s="43">
-        <v>0</v>
-      </c>
-      <c r="J5" s="16">
+      <c r="I5" s="31">
+        <v>0</v>
+      </c>
+      <c r="J5" s="14">
         <v>0</v>
       </c>
     </row>
@@ -1927,32 +1970,32 @@
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="41">
+      <c r="B6">
         <v>17706</v>
       </c>
-      <c r="C6" s="42">
+      <c r="C6" s="10">
         <f>$D6 * 1000000</f>
         <v>5696.7155999999995</v>
       </c>
-      <c r="D6" s="41">
+      <c r="D6">
         <v>5.6967156E-3</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6">
         <v>1560744</v>
       </c>
-      <c r="F6" s="41">
+      <c r="F6">
         <v>273.97260273972603</v>
       </c>
-      <c r="G6" s="43">
+      <c r="G6" s="31">
         <v>1.35781523642732E-2</v>
       </c>
-      <c r="H6" s="43">
+      <c r="H6" s="31">
         <v>1.6265323992994699E-2</v>
       </c>
-      <c r="I6" s="43">
-        <v>0</v>
-      </c>
-      <c r="J6" s="16">
+      <c r="I6" s="31">
+        <v>0</v>
+      </c>
+      <c r="J6" s="14">
         <v>0</v>
       </c>
     </row>
@@ -1960,117 +2003,122 @@
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="41">
+      <c r="B7">
         <v>17706</v>
       </c>
-      <c r="C7" s="42">
+      <c r="C7" s="10">
         <f t="shared" ref="C7:C9" si="0">$D7 * 1000000</f>
         <v>5696.7082999999993</v>
       </c>
-      <c r="D7" s="41">
+      <c r="D7">
         <v>5.6967082999999996E-3</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7">
         <v>1560742</v>
       </c>
-      <c r="F7" s="41">
+      <c r="F7">
         <v>273.97260273972603</v>
       </c>
-      <c r="G7" s="43">
+      <c r="G7" s="31">
         <v>3.0137186223000499E-3</v>
       </c>
-      <c r="H7" s="43">
+      <c r="H7" s="31">
         <v>9.8730297723292407E-3</v>
       </c>
-      <c r="I7" s="43">
-        <v>0</v>
-      </c>
-      <c r="J7" s="16">
+      <c r="I7" s="31">
+        <v>0</v>
+      </c>
+      <c r="J7" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>270074</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="20">
         <f t="shared" si="0"/>
         <v>1914.1877500000001</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>1.91418775E-3</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>524435</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>273.97260273972603</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="15">
         <v>7.8309252772912993E-2</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="15">
         <v>2.1555750145942701E-2</v>
       </c>
-      <c r="I8" s="17">
-        <v>0</v>
-      </c>
-      <c r="J8" s="18">
+      <c r="I8" s="15">
+        <v>0</v>
+      </c>
+      <c r="J8" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="8">
         <v>475604</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="11">
         <f t="shared" si="0"/>
         <v>17127.559300000001</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="17">
         <v>1.7127559300000001E-2</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="17">
         <v>4692482</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="17">
         <v>273.97260273972603</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="21">
         <v>6.9120329830706304E-2</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="21">
         <v>0.21306187974314</v>
       </c>
-      <c r="I9" s="23">
+      <c r="I9" s="21">
         <v>2.3947368421052602</v>
       </c>
-      <c r="J9" s="24">
+      <c r="J9" s="22">
         <v>1.03174603174603E-2</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="29" t="s">
+      <c r="E12" s="27" t="s">
         <v>30</v>
       </c>
+      <c r="G12" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="58"/>
+      <c r="I12" s="59"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -2082,13 +2130,22 @@
       <c r="C13" s="2">
         <v>4</v>
       </c>
-      <c r="D13" s="11">
-        <f>$B13*$C13*$B$20 + $B$21</f>
+      <c r="D13" s="9">
+        <f>$B13*$C13*$I$13 + $I$14</f>
         <v>4562.1665434388442</v>
       </c>
-      <c r="E13" s="30">
-        <f>$B13*$C13*$B$22 + $B$23</f>
+      <c r="E13" s="28">
+        <f>$B13*$C13*$I$15 + $I$16</f>
         <v>6671.5308280954259</v>
+      </c>
+      <c r="G13" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="68">
+        <v>1.4582852584745199E-3</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2101,13 +2158,20 @@
       <c r="C14">
         <v>4</v>
       </c>
-      <c r="D14" s="12">
-        <f t="shared" ref="D14:D17" si="1">$B14*$C14*$B$20 + $B$21</f>
-        <v>1503.9206970584871</v>
-      </c>
-      <c r="E14" s="31">
-        <f t="shared" ref="E14:E17" si="2">$B14*$C14*$B$22 + $B$23</f>
+      <c r="D14" s="10">
+        <f>$B14*$C14*$I$13 + $I$14</f>
+        <v>1503.9206970584871</v>
+      </c>
+      <c r="E14" s="29">
+        <f>$B14*$C14*$I$15 + $I$16</f>
         <v>2207.799534354021</v>
+      </c>
+      <c r="G14" s="56"/>
+      <c r="H14" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="69">
+        <v>-25.202226131690999</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2120,93 +2184,333 @@
       <c r="C15">
         <v>4</v>
       </c>
-      <c r="D15" s="12">
-        <f t="shared" si="1"/>
-        <v>1503.9206970584871</v>
-      </c>
-      <c r="E15" s="31">
-        <f t="shared" si="2"/>
+      <c r="D15" s="10">
+        <f>$B15*$C15*$I$13 + $I$14</f>
+        <v>1503.9206970584871</v>
+      </c>
+      <c r="E15" s="29">
+        <f>$B15*$C15*$I$15 + $I$16</f>
         <v>2207.799534354021</v>
       </c>
+      <c r="G15" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15" s="68">
+        <v>2.1284729450900099E-3</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16">
-        <v>9</v>
-      </c>
-      <c r="C16">
+      <c r="A16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="5">
+        <v>262144</v>
+      </c>
+      <c r="C16" s="5">
         <v>4</v>
       </c>
-      <c r="D16" s="12">
-        <f t="shared" si="1"/>
-        <v>-25.149727862385916</v>
-      </c>
-      <c r="E16" s="31">
-        <f t="shared" si="2"/>
-        <v>-23.989487490657858</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="6">
-        <v>262144</v>
-      </c>
-      <c r="C17" s="6">
-        <v>4</v>
-      </c>
-      <c r="D17" s="22">
-        <f t="shared" si="1"/>
-        <v>1503.9206970584871</v>
-      </c>
-      <c r="E17" s="32">
-        <f t="shared" si="2"/>
+      <c r="D16" s="20">
+        <f>$B16*$C16*$I$13 + $I$14</f>
+        <v>1503.9206970584871</v>
+      </c>
+      <c r="E16" s="30">
+        <f>$B16*$C16*$I$15 + $I$16</f>
         <v>2207.799534354021</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20">
-        <v>1.4582852584745199E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21">
-        <v>-25.202226131690999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22">
-        <v>2.1284729450900099E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23">
+      <c r="G16" s="56"/>
+      <c r="H16" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="I16" s="69">
         <v>-24.066112516681098</v>
       </c>
     </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="42"/>
+      <c r="B20" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20" s="41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="48">
+        <v>0</v>
+      </c>
+      <c r="C21" s="51">
+        <f>D14</f>
+        <v>1503.9206970584871</v>
+      </c>
+      <c r="D21" s="51">
+        <v>0</v>
+      </c>
+      <c r="E21" s="49">
+        <v>0</v>
+      </c>
+      <c r="F21" s="51">
+        <f>D15</f>
+        <v>1503.9206970584871</v>
+      </c>
+      <c r="G21" s="49">
+        <v>0</v>
+      </c>
+      <c r="H21" s="49">
+        <v>0</v>
+      </c>
+      <c r="I21" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="35">
+        <v>0</v>
+      </c>
+      <c r="C22" s="43">
+        <v>0</v>
+      </c>
+      <c r="D22" s="52">
+        <f>D14</f>
+        <v>1503.9206970584871</v>
+      </c>
+      <c r="E22" s="52">
+        <f>D14</f>
+        <v>1503.9206970584871</v>
+      </c>
+      <c r="F22" s="52">
+        <v>0</v>
+      </c>
+      <c r="G22" s="43">
+        <v>0</v>
+      </c>
+      <c r="H22" s="43">
+        <v>0</v>
+      </c>
+      <c r="I22" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="35">
+        <v>0</v>
+      </c>
+      <c r="C23" s="43">
+        <v>0</v>
+      </c>
+      <c r="D23" s="43">
+        <v>0</v>
+      </c>
+      <c r="E23" s="52">
+        <f>D16</f>
+        <v>1503.9206970584871</v>
+      </c>
+      <c r="F23" s="52">
+        <f>D16</f>
+        <v>1503.9206970584871</v>
+      </c>
+      <c r="G23" s="52">
+        <f>D14</f>
+        <v>1503.9206970584871</v>
+      </c>
+      <c r="H23" s="43">
+        <v>0</v>
+      </c>
+      <c r="I23" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="35">
+        <v>0</v>
+      </c>
+      <c r="C24" s="43">
+        <v>0</v>
+      </c>
+      <c r="D24" s="43">
+        <v>0</v>
+      </c>
+      <c r="E24" s="43">
+        <v>0</v>
+      </c>
+      <c r="F24" s="52">
+        <v>0</v>
+      </c>
+      <c r="G24" s="52">
+        <f>D16</f>
+        <v>1503.9206970584871</v>
+      </c>
+      <c r="H24" s="43">
+        <v>0</v>
+      </c>
+      <c r="I24" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="35">
+        <v>0</v>
+      </c>
+      <c r="C25" s="43">
+        <v>0</v>
+      </c>
+      <c r="D25" s="43">
+        <v>0</v>
+      </c>
+      <c r="E25" s="43">
+        <v>0</v>
+      </c>
+      <c r="F25" s="43">
+        <v>0</v>
+      </c>
+      <c r="G25" s="52">
+        <f>D15</f>
+        <v>1503.9206970584871</v>
+      </c>
+      <c r="H25" s="43">
+        <v>0</v>
+      </c>
+      <c r="I25" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="35">
+        <v>0</v>
+      </c>
+      <c r="C26" s="52">
+        <v>0</v>
+      </c>
+      <c r="D26" s="43">
+        <v>0</v>
+      </c>
+      <c r="E26" s="43">
+        <v>0</v>
+      </c>
+      <c r="F26" s="43">
+        <v>0</v>
+      </c>
+      <c r="G26" s="43">
+        <v>0</v>
+      </c>
+      <c r="H26" s="43">
+        <v>0</v>
+      </c>
+      <c r="I26" s="53">
+        <f>D16</f>
+        <v>1503.9206970584871</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="54">
+        <v>0</v>
+      </c>
+      <c r="C27" s="52">
+        <f>D13</f>
+        <v>4562.1665434388442</v>
+      </c>
+      <c r="D27" s="52">
+        <f>D16</f>
+        <v>1503.9206970584871</v>
+      </c>
+      <c r="E27" s="52">
+        <v>0</v>
+      </c>
+      <c r="F27" s="43">
+        <v>0</v>
+      </c>
+      <c r="G27" s="52">
+        <v>0</v>
+      </c>
+      <c r="H27" s="43">
+        <v>0</v>
+      </c>
+      <c r="I27" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="36">
+        <v>0</v>
+      </c>
+      <c r="C28" s="45">
+        <v>0</v>
+      </c>
+      <c r="D28" s="45">
+        <v>0</v>
+      </c>
+      <c r="E28" s="45">
+        <v>0</v>
+      </c>
+      <c r="F28" s="45">
+        <v>0</v>
+      </c>
+      <c r="G28" s="45">
+        <v>0</v>
+      </c>
+      <c r="H28" s="45">
+        <v>0</v>
+      </c>
+      <c r="I28" s="46">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="G15:G16"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:J1"/>
+    <mergeCell ref="G12:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New image sizes for generic ED
</commit_message>
<xml_diff>
--- a/TaskgraphsEdgeDetect/hwsw-partitioning/TaskGraph-Attributes.xlsx
+++ b/TaskgraphsEdgeDetect/hwsw-partitioning/TaskGraph-Attributes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Dev\Experiments\TaskgraphsEdgeDetect\hwsw-partitioning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D5B146-117D-4D60-9DDE-A810A64D2DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D0F12C-546C-4B84-8DA0-D5E0693360AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1806,7 +1806,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="B21" sqref="B21:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Jetson results for ED
</commit_message>
<xml_diff>
--- a/TaskgraphsEdgeDetect/hwsw-partitioning/TaskGraph-Attributes.xlsx
+++ b/TaskgraphsEdgeDetect/hwsw-partitioning/TaskGraph-Attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Dev\Experiments\TaskgraphsEdgeDetect\hwsw-partitioning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D0F12C-546C-4B84-8DA0-D5E0693360AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8022F8-1986-42D0-B964-D4B0B0697A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V0" sheetId="1" r:id="rId1"/>
@@ -414,14 +414,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -459,7 +458,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -508,48 +506,49 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -943,7 +942,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,48 +959,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="62"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="63"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="23" t="s">
+      <c r="A2" s="64"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="23" t="s">
+      <c r="E2" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="23" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1012,11 +1011,12 @@
       <c r="B3" s="2">
         <v>143601</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <f>$D3 * 1000000</f>
         <v>2871.1593500000004</v>
       </c>
       <c r="D3" s="2">
+        <f>$E3/($F3*1000000)</f>
         <v>2.8711593500000002E-3</v>
       </c>
       <c r="E3" s="2">
@@ -1025,16 +1025,16 @@
       <c r="F3" s="2">
         <v>273.97260273972603</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="11">
         <v>1.3271672504378201E-2</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="11">
         <v>5.0492556917688197E-2</v>
       </c>
-      <c r="I3" s="12">
-        <v>0</v>
-      </c>
-      <c r="J3" s="13">
+      <c r="I3" s="11">
+        <v>0</v>
+      </c>
+      <c r="J3" s="12">
         <v>5.5555555555555497E-3</v>
       </c>
     </row>
@@ -1045,11 +1045,12 @@
       <c r="B4">
         <v>14467</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <f t="shared" ref="C4:C9" si="0">$D4 * 1000000</f>
         <v>8546.0698500000017</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="69">
+        <f t="shared" ref="D4:D9" si="1">$E4/($F4*1000000)</f>
         <v>8.5460698500000008E-3</v>
       </c>
       <c r="E4">
@@ -1058,16 +1059,16 @@
       <c r="F4">
         <v>273.97260273972603</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="30">
         <v>2.6514156450671299E-2</v>
       </c>
-      <c r="H4" s="31">
+      <c r="H4" s="30">
         <v>0.133413601868067</v>
       </c>
-      <c r="I4" s="31">
-        <v>0</v>
-      </c>
-      <c r="J4" s="14">
+      <c r="I4" s="30">
+        <v>0</v>
+      </c>
+      <c r="J4" s="13">
         <v>1.0714285714285701E-2</v>
       </c>
     </row>
@@ -1078,12 +1079,13 @@
       <c r="B5">
         <v>245034</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <f t="shared" si="0"/>
-        <v>1914.1877500000001</v>
-      </c>
-      <c r="D5">
-        <v>1.91418775E-3</v>
+        <v>1914.1877500000003</v>
+      </c>
+      <c r="D5" s="69">
+        <f t="shared" si="1"/>
+        <v>1.9141877500000002E-3</v>
       </c>
       <c r="E5">
         <v>524435</v>
@@ -1091,16 +1093,16 @@
       <c r="F5">
         <v>273.97260273972603</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="30">
         <v>7.8309252772912993E-2</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="30">
         <v>2.1555750145942701E-2</v>
       </c>
-      <c r="I5" s="31">
-        <v>0</v>
-      </c>
-      <c r="J5" s="14">
+      <c r="I5" s="30">
+        <v>0</v>
+      </c>
+      <c r="J5" s="13">
         <v>0</v>
       </c>
     </row>
@@ -1111,12 +1113,13 @@
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <f t="shared" si="0"/>
         <v>0.2555</v>
       </c>
-      <c r="D6" s="32">
-        <v>2.5549999999999998E-7</v>
+      <c r="D6" s="69">
+        <f t="shared" si="1"/>
+        <v>2.5550000000000003E-7</v>
       </c>
       <c r="E6">
         <v>70</v>
@@ -1124,16 +1127,16 @@
       <c r="F6">
         <v>273.97260273972603</v>
       </c>
-      <c r="G6" s="31">
+      <c r="G6" s="30">
         <v>3.3785755983654401E-3</v>
       </c>
-      <c r="H6" s="31">
+      <c r="H6" s="30">
         <v>1.0402072387624001E-2</v>
       </c>
-      <c r="I6" s="31">
-        <v>0</v>
-      </c>
-      <c r="J6" s="14">
+      <c r="I6" s="30">
+        <v>0</v>
+      </c>
+      <c r="J6" s="13">
         <v>0</v>
       </c>
     </row>
@@ -1144,12 +1147,13 @@
       <c r="B7">
         <v>0</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <f t="shared" si="0"/>
         <v>0.2555</v>
       </c>
-      <c r="D7" s="32">
-        <v>2.5549999999999998E-7</v>
+      <c r="D7" s="69">
+        <f t="shared" si="1"/>
+        <v>2.5550000000000003E-7</v>
       </c>
       <c r="E7">
         <v>70</v>
@@ -1157,16 +1161,16 @@
       <c r="F7">
         <v>273.97260273972603</v>
       </c>
-      <c r="G7" s="31">
+      <c r="G7" s="30">
         <v>3.3785755983654401E-3</v>
       </c>
-      <c r="H7" s="31">
+      <c r="H7" s="30">
         <v>1.0402072387624001E-2</v>
       </c>
-      <c r="I7" s="31">
-        <v>0</v>
-      </c>
-      <c r="J7" s="14">
+      <c r="I7" s="30">
+        <v>0</v>
+      </c>
+      <c r="J7" s="13">
         <v>0</v>
       </c>
     </row>
@@ -1177,12 +1181,13 @@
       <c r="B8" s="5">
         <v>0</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="19">
         <f t="shared" si="0"/>
         <v>0.2555</v>
       </c>
-      <c r="D8" s="6">
-        <v>2.5549999999999998E-7</v>
+      <c r="D8" s="69">
+        <f t="shared" si="1"/>
+        <v>2.5550000000000003E-7</v>
       </c>
       <c r="E8" s="5">
         <v>70</v>
@@ -1190,73 +1195,74 @@
       <c r="F8" s="5">
         <v>273.97260273972603</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="14">
         <v>3.3785755983654401E-3</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="14">
         <v>1.0402072387624001E-2</v>
       </c>
-      <c r="I8" s="15">
-        <v>0</v>
-      </c>
-      <c r="J8" s="16">
+      <c r="I8" s="14">
+        <v>0</v>
+      </c>
+      <c r="J8" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="7">
         <v>435372</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <f t="shared" si="0"/>
         <v>534535.19634999998</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="7">
+        <f t="shared" si="1"/>
         <v>0.53453519635000002</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <v>146447999</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="7">
         <v>273.97260273972603</v>
       </c>
-      <c r="G9" s="33">
+      <c r="G9" s="31">
         <v>0.11206217162872099</v>
       </c>
-      <c r="H9" s="33">
+      <c r="H9" s="31">
         <v>0.19555239346176201</v>
       </c>
-      <c r="I9" s="33">
-        <v>0</v>
-      </c>
-      <c r="J9" s="34">
+      <c r="I9" s="31">
+        <v>0</v>
+      </c>
+      <c r="J9" s="32">
         <v>1.6269841269841202E-2</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="57" t="s">
+      <c r="G12" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="58"/>
-      <c r="I12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="60"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1268,21 +1274,21 @@
       <c r="C13" s="2">
         <v>4</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <f>$B13*$C13*$I$13 + $I$14</f>
         <v>4562.1665434388442</v>
       </c>
-      <c r="E13" s="28">
+      <c r="E13" s="27">
         <f>$B13*$C13*$I$15 + $I$16</f>
         <v>6671.5308280954259</v>
       </c>
-      <c r="G13" s="55" t="s">
+      <c r="G13" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="35" t="s">
+      <c r="H13" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="I13" s="68">
+      <c r="I13" s="53">
         <v>1.4582852584745199E-3</v>
       </c>
     </row>
@@ -1296,19 +1302,19 @@
       <c r="C14">
         <v>4</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <f>$B14*$C14*$I$13 + $I$14</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E14" s="28">
         <f>$B14*$C14*$I$15 + $I$16</f>
         <v>2207.799534354021</v>
       </c>
-      <c r="G14" s="56"/>
-      <c r="H14" s="36" t="s">
+      <c r="G14" s="57"/>
+      <c r="H14" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="69">
+      <c r="I14" s="54">
         <v>-25.202226131690999</v>
       </c>
     </row>
@@ -1322,21 +1328,21 @@
       <c r="C15">
         <v>4</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="9">
         <f>$B15*$C15*$I$13 + $I$14</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="28">
         <f>$B15*$C15*$I$15 + $I$16</f>
         <v>2207.799534354021</v>
       </c>
-      <c r="G15" s="55" t="s">
+      <c r="G15" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="35" t="s">
+      <c r="H15" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="I15" s="70">
+      <c r="I15" s="55">
         <v>2.1284729450900099E-3</v>
       </c>
     </row>
@@ -1350,19 +1356,19 @@
       <c r="C16">
         <v>4</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="9">
         <f>$B16*$C16*$I$13 + $I$14</f>
         <v>-25.149727862385916</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="28">
         <f>$B16*$C16*$I$15 + $I$16</f>
         <v>-23.989487490657858</v>
       </c>
-      <c r="G16" s="56"/>
-      <c r="H16" s="36" t="s">
+      <c r="G16" s="57"/>
+      <c r="H16" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="I16" s="69">
+      <c r="I16" s="54">
         <v>-24.066112516681098</v>
       </c>
     </row>
@@ -1376,412 +1382,412 @@
       <c r="C17" s="5">
         <v>4</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="19">
         <f>$B17*$C17*$I$13 + $I$14</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="E17" s="30">
+      <c r="E17" s="29">
         <f>$B17*$C17*$I$15 + $I$16</f>
         <v>2207.799534354021</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="42"/>
-      <c r="B20" s="47" t="s">
+      <c r="A20" s="40"/>
+      <c r="B20" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="40" t="s">
+      <c r="D20" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="40" t="s">
+      <c r="E20" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="40" t="s">
+      <c r="F20" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="40" t="s">
+      <c r="G20" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="40" t="s">
+      <c r="H20" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="I20" s="40" t="s">
+      <c r="I20" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="J20" s="40" t="s">
+      <c r="J20" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="K20" s="41" t="s">
+      <c r="K20" s="39" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="48">
-        <v>0</v>
-      </c>
-      <c r="C21" s="51">
+      <c r="B21" s="46">
+        <v>0</v>
+      </c>
+      <c r="C21" s="49">
         <f>D14</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="D21" s="51">
+      <c r="D21" s="49">
         <f>D14</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="E21" s="49">
-        <v>0</v>
-      </c>
-      <c r="F21" s="49">
-        <v>0</v>
-      </c>
-      <c r="G21" s="49">
-        <v>0</v>
-      </c>
-      <c r="H21" s="49">
-        <v>0</v>
-      </c>
-      <c r="I21" s="49">
-        <v>0</v>
-      </c>
-      <c r="J21" s="49">
-        <v>0</v>
-      </c>
-      <c r="K21" s="50">
+      <c r="E21" s="47">
+        <v>0</v>
+      </c>
+      <c r="F21" s="47">
+        <v>0</v>
+      </c>
+      <c r="G21" s="47">
+        <v>0</v>
+      </c>
+      <c r="H21" s="47">
+        <v>0</v>
+      </c>
+      <c r="I21" s="47">
+        <v>0</v>
+      </c>
+      <c r="J21" s="47">
+        <v>0</v>
+      </c>
+      <c r="K21" s="48">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="35">
-        <v>0</v>
-      </c>
-      <c r="C22" s="43">
-        <v>0</v>
-      </c>
-      <c r="D22" s="52">
+      <c r="B22" s="33">
+        <v>0</v>
+      </c>
+      <c r="C22" s="41">
+        <v>0</v>
+      </c>
+      <c r="D22" s="50">
         <f>D17</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="E22" s="52">
+      <c r="E22" s="50">
         <f>D17</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="F22" s="52">
+      <c r="F22" s="50">
         <f>D17</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="G22" s="43">
-        <v>0</v>
-      </c>
-      <c r="H22" s="43">
-        <v>0</v>
-      </c>
-      <c r="I22" s="43">
-        <v>0</v>
-      </c>
-      <c r="J22" s="43">
-        <v>0</v>
-      </c>
-      <c r="K22" s="44">
+      <c r="G22" s="41">
+        <v>0</v>
+      </c>
+      <c r="H22" s="41">
+        <v>0</v>
+      </c>
+      <c r="I22" s="41">
+        <v>0</v>
+      </c>
+      <c r="J22" s="41">
+        <v>0</v>
+      </c>
+      <c r="K22" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="35">
-        <v>0</v>
-      </c>
-      <c r="C23" s="43">
-        <v>0</v>
-      </c>
-      <c r="D23" s="43">
-        <v>0</v>
-      </c>
-      <c r="E23" s="43">
-        <v>0</v>
-      </c>
-      <c r="F23" s="52">
+      <c r="B23" s="33">
+        <v>0</v>
+      </c>
+      <c r="C23" s="41">
+        <v>0</v>
+      </c>
+      <c r="D23" s="41">
+        <v>0</v>
+      </c>
+      <c r="E23" s="41">
+        <v>0</v>
+      </c>
+      <c r="F23" s="50">
         <f>D14</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="G23" s="43">
-        <v>0</v>
-      </c>
-      <c r="H23" s="43">
-        <v>0</v>
-      </c>
-      <c r="I23" s="43">
-        <v>0</v>
-      </c>
-      <c r="J23" s="43">
-        <v>0</v>
-      </c>
-      <c r="K23" s="44">
+      <c r="G23" s="41">
+        <v>0</v>
+      </c>
+      <c r="H23" s="41">
+        <v>0</v>
+      </c>
+      <c r="I23" s="41">
+        <v>0</v>
+      </c>
+      <c r="J23" s="41">
+        <v>0</v>
+      </c>
+      <c r="K23" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="35">
-        <v>0</v>
-      </c>
-      <c r="C24" s="43">
-        <v>0</v>
-      </c>
-      <c r="D24" s="43">
-        <v>0</v>
-      </c>
-      <c r="E24" s="43">
-        <v>0</v>
-      </c>
-      <c r="F24" s="52">
+      <c r="B24" s="33">
+        <v>0</v>
+      </c>
+      <c r="C24" s="41">
+        <v>0</v>
+      </c>
+      <c r="D24" s="41">
+        <v>0</v>
+      </c>
+      <c r="E24" s="41">
+        <v>0</v>
+      </c>
+      <c r="F24" s="50">
         <f>D15</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="G24" s="43">
-        <v>0</v>
-      </c>
-      <c r="H24" s="43">
-        <v>0</v>
-      </c>
-      <c r="I24" s="43">
-        <v>0</v>
-      </c>
-      <c r="J24" s="43">
-        <v>0</v>
-      </c>
-      <c r="K24" s="44">
+      <c r="G24" s="41">
+        <v>0</v>
+      </c>
+      <c r="H24" s="41">
+        <v>0</v>
+      </c>
+      <c r="I24" s="41">
+        <v>0</v>
+      </c>
+      <c r="J24" s="41">
+        <v>0</v>
+      </c>
+      <c r="K24" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="35">
-        <v>0</v>
-      </c>
-      <c r="C25" s="43">
-        <v>0</v>
-      </c>
-      <c r="D25" s="43">
-        <v>0</v>
-      </c>
-      <c r="E25" s="43">
-        <v>0</v>
-      </c>
-      <c r="F25" s="43">
-        <v>0</v>
-      </c>
-      <c r="G25" s="43">
-        <v>0</v>
-      </c>
-      <c r="H25" s="43">
-        <v>0</v>
-      </c>
-      <c r="I25" s="43">
-        <v>0</v>
-      </c>
-      <c r="J25" s="43">
-        <v>0</v>
-      </c>
-      <c r="K25" s="53">
+      <c r="B25" s="33">
+        <v>0</v>
+      </c>
+      <c r="C25" s="41">
+        <v>0</v>
+      </c>
+      <c r="D25" s="41">
+        <v>0</v>
+      </c>
+      <c r="E25" s="41">
+        <v>0</v>
+      </c>
+      <c r="F25" s="41">
+        <v>0</v>
+      </c>
+      <c r="G25" s="41">
+        <v>0</v>
+      </c>
+      <c r="H25" s="41">
+        <v>0</v>
+      </c>
+      <c r="I25" s="41">
+        <v>0</v>
+      </c>
+      <c r="J25" s="41">
+        <v>0</v>
+      </c>
+      <c r="K25" s="51">
         <f>D17</f>
         <v>1503.9206970584871</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="35">
-        <v>0</v>
-      </c>
-      <c r="C26" s="52">
+      <c r="B26" s="33">
+        <v>0</v>
+      </c>
+      <c r="C26" s="50">
         <f>D16</f>
         <v>-25.149727862385916</v>
       </c>
-      <c r="D26" s="43">
-        <v>0</v>
-      </c>
-      <c r="E26" s="43">
-        <v>0</v>
-      </c>
-      <c r="F26" s="43">
-        <v>0</v>
-      </c>
-      <c r="G26" s="43">
-        <v>0</v>
-      </c>
-      <c r="H26" s="52">
+      <c r="D26" s="41">
+        <v>0</v>
+      </c>
+      <c r="E26" s="41">
+        <v>0</v>
+      </c>
+      <c r="F26" s="41">
+        <v>0</v>
+      </c>
+      <c r="G26" s="41">
+        <v>0</v>
+      </c>
+      <c r="H26" s="50">
         <f>D16</f>
         <v>-25.149727862385916</v>
       </c>
-      <c r="I26" s="43">
-        <v>0</v>
-      </c>
-      <c r="J26" s="43">
-        <v>0</v>
-      </c>
-      <c r="K26" s="44">
+      <c r="I26" s="41">
+        <v>0</v>
+      </c>
+      <c r="J26" s="41">
+        <v>0</v>
+      </c>
+      <c r="K26" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="35">
-        <v>0</v>
-      </c>
-      <c r="C27" s="43">
-        <v>0</v>
-      </c>
-      <c r="D27" s="52">
+      <c r="B27" s="33">
+        <v>0</v>
+      </c>
+      <c r="C27" s="41">
+        <v>0</v>
+      </c>
+      <c r="D27" s="50">
         <f>D16</f>
         <v>-25.149727862385916</v>
       </c>
-      <c r="E27" s="43">
-        <v>0</v>
-      </c>
-      <c r="F27" s="43">
-        <v>0</v>
-      </c>
-      <c r="G27" s="43">
-        <v>0</v>
-      </c>
-      <c r="H27" s="43">
-        <v>0</v>
-      </c>
-      <c r="I27" s="52">
+      <c r="E27" s="41">
+        <v>0</v>
+      </c>
+      <c r="F27" s="41">
+        <v>0</v>
+      </c>
+      <c r="G27" s="41">
+        <v>0</v>
+      </c>
+      <c r="H27" s="41">
+        <v>0</v>
+      </c>
+      <c r="I27" s="50">
         <f>D16</f>
         <v>-25.149727862385916</v>
       </c>
-      <c r="J27" s="43">
-        <v>0</v>
-      </c>
-      <c r="K27" s="44">
+      <c r="J27" s="41">
+        <v>0</v>
+      </c>
+      <c r="K27" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="35">
-        <v>0</v>
-      </c>
-      <c r="C28" s="43">
-        <v>0</v>
-      </c>
-      <c r="D28" s="43">
-        <v>0</v>
-      </c>
-      <c r="E28" s="52">
+      <c r="B28" s="33">
+        <v>0</v>
+      </c>
+      <c r="C28" s="41">
+        <v>0</v>
+      </c>
+      <c r="D28" s="41">
+        <v>0</v>
+      </c>
+      <c r="E28" s="50">
         <f>D16</f>
         <v>-25.149727862385916</v>
       </c>
-      <c r="F28" s="43">
-        <v>0</v>
-      </c>
-      <c r="G28" s="43">
-        <v>0</v>
-      </c>
-      <c r="H28" s="43">
-        <v>0</v>
-      </c>
-      <c r="I28" s="43">
-        <v>0</v>
-      </c>
-      <c r="J28" s="43">
-        <v>0</v>
-      </c>
-      <c r="K28" s="44">
+      <c r="F28" s="41">
+        <v>0</v>
+      </c>
+      <c r="G28" s="41">
+        <v>0</v>
+      </c>
+      <c r="H28" s="41">
+        <v>0</v>
+      </c>
+      <c r="I28" s="41">
+        <v>0</v>
+      </c>
+      <c r="J28" s="41">
+        <v>0</v>
+      </c>
+      <c r="K28" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="54">
+      <c r="B29" s="52">
         <f>D13+D14</f>
         <v>6066.0872404973315</v>
       </c>
-      <c r="C29" s="52">
+      <c r="C29" s="50">
         <f>D17</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="D29" s="43">
-        <v>0</v>
-      </c>
-      <c r="E29" s="52">
+      <c r="D29" s="41">
+        <v>0</v>
+      </c>
+      <c r="E29" s="50">
         <f>D15</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="F29" s="43">
-        <v>0</v>
-      </c>
-      <c r="G29" s="52">
+      <c r="F29" s="41">
+        <v>0</v>
+      </c>
+      <c r="G29" s="50">
         <f>D16</f>
         <v>-25.149727862385916</v>
       </c>
-      <c r="H29" s="43">
-        <v>0</v>
-      </c>
-      <c r="I29" s="43">
-        <v>0</v>
-      </c>
-      <c r="J29" s="43">
-        <v>0</v>
-      </c>
-      <c r="K29" s="44">
+      <c r="H29" s="41">
+        <v>0</v>
+      </c>
+      <c r="I29" s="41">
+        <v>0</v>
+      </c>
+      <c r="J29" s="41">
+        <v>0</v>
+      </c>
+      <c r="K29" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="36">
-        <v>0</v>
-      </c>
-      <c r="C30" s="45">
-        <v>0</v>
-      </c>
-      <c r="D30" s="45">
-        <v>0</v>
-      </c>
-      <c r="E30" s="45">
-        <v>0</v>
-      </c>
-      <c r="F30" s="45">
-        <v>0</v>
-      </c>
-      <c r="G30" s="45">
-        <v>0</v>
-      </c>
-      <c r="H30" s="45">
-        <v>0</v>
-      </c>
-      <c r="I30" s="45">
-        <v>0</v>
-      </c>
-      <c r="J30" s="45">
-        <v>0</v>
-      </c>
-      <c r="K30" s="46">
+      <c r="B30" s="34">
+        <v>0</v>
+      </c>
+      <c r="C30" s="43">
+        <v>0</v>
+      </c>
+      <c r="D30" s="43">
+        <v>0</v>
+      </c>
+      <c r="E30" s="43">
+        <v>0</v>
+      </c>
+      <c r="F30" s="43">
+        <v>0</v>
+      </c>
+      <c r="G30" s="43">
+        <v>0</v>
+      </c>
+      <c r="H30" s="43">
+        <v>0</v>
+      </c>
+      <c r="I30" s="43">
+        <v>0</v>
+      </c>
+      <c r="J30" s="43">
+        <v>0</v>
+      </c>
+      <c r="K30" s="44">
         <v>0</v>
       </c>
     </row>
@@ -1806,7 +1812,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:I28"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1823,48 +1829,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="62"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="63"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="23" t="s">
+      <c r="A2" s="64"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="23" t="s">
+      <c r="E2" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="23" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1872,31 +1878,31 @@
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="18" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1907,11 +1913,12 @@
       <c r="B4">
         <v>149827</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <f>$D4 * 1000000</f>
         <v>2871.1593500000004</v>
       </c>
       <c r="D4">
+        <f>$E4/($F4*1000000)</f>
         <v>2.8711593500000002E-3</v>
       </c>
       <c r="E4">
@@ -1920,16 +1927,16 @@
       <c r="F4">
         <v>273.97260273972603</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="30">
         <v>1.3271672504378201E-2</v>
       </c>
-      <c r="H4" s="31">
+      <c r="H4" s="30">
         <v>5.0492556917688197E-2</v>
       </c>
-      <c r="I4" s="31">
-        <v>0</v>
-      </c>
-      <c r="J4" s="14">
+      <c r="I4" s="30">
+        <v>0</v>
+      </c>
+      <c r="J4" s="13">
         <v>5.5555555555555497E-3</v>
       </c>
     </row>
@@ -1940,11 +1947,12 @@
       <c r="B5">
         <v>17706</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <f>$D5 * 1000000</f>
         <v>8544.8069500000001</v>
       </c>
       <c r="D5">
+        <f t="shared" ref="D5:D9" si="0">$E5/($F5*1000000)</f>
         <v>8.5448069500000008E-3</v>
       </c>
       <c r="E5">
@@ -1953,16 +1961,16 @@
       <c r="F5">
         <v>273.97260273972603</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="30">
         <v>3.3986427320490298E-3</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="30">
         <v>1.04057209573847E-2</v>
       </c>
-      <c r="I5" s="31">
-        <v>0</v>
-      </c>
-      <c r="J5" s="14">
+      <c r="I5" s="30">
+        <v>0</v>
+      </c>
+      <c r="J5" s="13">
         <v>0</v>
       </c>
     </row>
@@ -1973,12 +1981,13 @@
       <c r="B6">
         <v>17706</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <f>$D6 * 1000000</f>
-        <v>5696.7155999999995</v>
+        <v>5696.7156000000004</v>
       </c>
       <c r="D6">
-        <v>5.6967156E-3</v>
+        <f t="shared" si="0"/>
+        <v>5.6967156000000008E-3</v>
       </c>
       <c r="E6">
         <v>1560744</v>
@@ -1986,16 +1995,16 @@
       <c r="F6">
         <v>273.97260273972603</v>
       </c>
-      <c r="G6" s="31">
+      <c r="G6" s="30">
         <v>1.35781523642732E-2</v>
       </c>
-      <c r="H6" s="31">
+      <c r="H6" s="30">
         <v>1.6265323992994699E-2</v>
       </c>
-      <c r="I6" s="31">
-        <v>0</v>
-      </c>
-      <c r="J6" s="14">
+      <c r="I6" s="30">
+        <v>0</v>
+      </c>
+      <c r="J6" s="13">
         <v>0</v>
       </c>
     </row>
@@ -2006,12 +2015,13 @@
       <c r="B7">
         <v>17706</v>
       </c>
-      <c r="C7" s="10">
-        <f t="shared" ref="C7:C9" si="0">$D7 * 1000000</f>
-        <v>5696.7082999999993</v>
+      <c r="C7" s="9">
+        <f t="shared" ref="C7:C9" si="1">$D7 * 1000000</f>
+        <v>5696.7083000000002</v>
       </c>
       <c r="D7">
-        <v>5.6967082999999996E-3</v>
+        <f t="shared" si="0"/>
+        <v>5.6967083000000005E-3</v>
       </c>
       <c r="E7">
         <v>1560742</v>
@@ -2019,16 +2029,16 @@
       <c r="F7">
         <v>273.97260273972603</v>
       </c>
-      <c r="G7" s="31">
+      <c r="G7" s="30">
         <v>3.0137186223000499E-3</v>
       </c>
-      <c r="H7" s="31">
+      <c r="H7" s="30">
         <v>9.8730297723292407E-3</v>
       </c>
-      <c r="I7" s="31">
-        <v>0</v>
-      </c>
-      <c r="J7" s="14">
+      <c r="I7" s="30">
+        <v>0</v>
+      </c>
+      <c r="J7" s="13">
         <v>0</v>
       </c>
     </row>
@@ -2039,12 +2049,13 @@
       <c r="B8" s="5">
         <v>270074</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="19">
+        <f t="shared" si="1"/>
+        <v>1914.1877500000003</v>
+      </c>
+      <c r="D8">
         <f t="shared" si="0"/>
-        <v>1914.1877500000001</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1.91418775E-3</v>
+        <v>1.9141877500000002E-3</v>
       </c>
       <c r="E8" s="5">
         <v>524435</v>
@@ -2052,73 +2063,74 @@
       <c r="F8" s="5">
         <v>273.97260273972603</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="14">
         <v>7.8309252772912993E-2</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="14">
         <v>2.1555750145942701E-2</v>
       </c>
-      <c r="I8" s="15">
-        <v>0</v>
-      </c>
-      <c r="J8" s="16">
+      <c r="I8" s="14">
+        <v>0</v>
+      </c>
+      <c r="J8" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="7">
         <v>475604</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10">
+        <f t="shared" si="1"/>
+        <v>17127.559300000001</v>
+      </c>
+      <c r="D9" s="7">
         <f t="shared" si="0"/>
-        <v>17127.559300000001</v>
-      </c>
-      <c r="D9" s="17">
         <v>1.7127559300000001E-2</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="16">
         <v>4692482</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="16">
         <v>273.97260273972603</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="20">
         <v>6.9120329830706304E-2</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="20">
         <v>0.21306187974314</v>
       </c>
-      <c r="I9" s="21">
+      <c r="I9" s="20">
         <v>2.3947368421052602</v>
       </c>
-      <c r="J9" s="22">
+      <c r="J9" s="21">
         <v>1.03174603174603E-2</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="57" t="s">
+      <c r="G12" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="58"/>
-      <c r="I12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="60"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -2130,21 +2142,21 @@
       <c r="C13" s="2">
         <v>4</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <f>$B13*$C13*$I$13 + $I$14</f>
         <v>4562.1665434388442</v>
       </c>
-      <c r="E13" s="28">
+      <c r="E13" s="27">
         <f>$B13*$C13*$I$15 + $I$16</f>
         <v>6671.5308280954259</v>
       </c>
-      <c r="G13" s="55" t="s">
+      <c r="G13" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="35" t="s">
+      <c r="H13" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="I13" s="68">
+      <c r="I13" s="53">
         <v>1.4582852584745199E-3</v>
       </c>
     </row>
@@ -2158,19 +2170,19 @@
       <c r="C14">
         <v>4</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <f>$B14*$C14*$I$13 + $I$14</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E14" s="28">
         <f>$B14*$C14*$I$15 + $I$16</f>
         <v>2207.799534354021</v>
       </c>
-      <c r="G14" s="56"/>
-      <c r="H14" s="36" t="s">
+      <c r="G14" s="57"/>
+      <c r="H14" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="69">
+      <c r="I14" s="54">
         <v>-25.202226131690999</v>
       </c>
     </row>
@@ -2184,21 +2196,21 @@
       <c r="C15">
         <v>4</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="9">
         <f>$B15*$C15*$I$13 + $I$14</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="28">
         <f>$B15*$C15*$I$15 + $I$16</f>
         <v>2207.799534354021</v>
       </c>
-      <c r="G15" s="55" t="s">
+      <c r="G15" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="35" t="s">
+      <c r="H15" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="I15" s="68">
+      <c r="I15" s="53">
         <v>2.1284729450900099E-3</v>
       </c>
     </row>
@@ -2212,290 +2224,290 @@
       <c r="C16" s="5">
         <v>4</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D16" s="19">
         <f>$B16*$C16*$I$13 + $I$14</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="E16" s="30">
+      <c r="E16" s="29">
         <f>$B16*$C16*$I$15 + $I$16</f>
         <v>2207.799534354021</v>
       </c>
-      <c r="G16" s="56"/>
-      <c r="H16" s="36" t="s">
+      <c r="G16" s="57"/>
+      <c r="H16" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="I16" s="69">
+      <c r="I16" s="54">
         <v>-24.066112516681098</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="42"/>
-      <c r="B20" s="47" t="s">
+      <c r="A20" s="40"/>
+      <c r="B20" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="40" t="s">
+      <c r="D20" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="40" t="s">
+      <c r="E20" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="40" t="s">
+      <c r="F20" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="40" t="s">
+      <c r="G20" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="H20" s="40" t="s">
+      <c r="H20" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="I20" s="41" t="s">
+      <c r="I20" s="39" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="48">
-        <v>0</v>
-      </c>
-      <c r="C21" s="51">
+      <c r="B21" s="46">
+        <v>0</v>
+      </c>
+      <c r="C21" s="49">
         <f>D14</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="D21" s="51">
-        <v>0</v>
-      </c>
-      <c r="E21" s="49">
-        <v>0</v>
-      </c>
-      <c r="F21" s="51">
+      <c r="D21" s="49">
+        <v>0</v>
+      </c>
+      <c r="E21" s="47">
+        <v>0</v>
+      </c>
+      <c r="F21" s="49">
         <f>D15</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="G21" s="49">
-        <v>0</v>
-      </c>
-      <c r="H21" s="49">
-        <v>0</v>
-      </c>
-      <c r="I21" s="50">
+      <c r="G21" s="47">
+        <v>0</v>
+      </c>
+      <c r="H21" s="47">
+        <v>0</v>
+      </c>
+      <c r="I21" s="48">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="35">
-        <v>0</v>
-      </c>
-      <c r="C22" s="43">
-        <v>0</v>
-      </c>
-      <c r="D22" s="52">
+      <c r="B22" s="33">
+        <v>0</v>
+      </c>
+      <c r="C22" s="41">
+        <v>0</v>
+      </c>
+      <c r="D22" s="50">
         <f>D14</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="E22" s="52">
+      <c r="E22" s="50">
         <f>D14</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="F22" s="52">
-        <v>0</v>
-      </c>
-      <c r="G22" s="43">
-        <v>0</v>
-      </c>
-      <c r="H22" s="43">
-        <v>0</v>
-      </c>
-      <c r="I22" s="44">
+      <c r="F22" s="50">
+        <v>0</v>
+      </c>
+      <c r="G22" s="41">
+        <v>0</v>
+      </c>
+      <c r="H22" s="41">
+        <v>0</v>
+      </c>
+      <c r="I22" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="35">
-        <v>0</v>
-      </c>
-      <c r="C23" s="43">
-        <v>0</v>
-      </c>
-      <c r="D23" s="43">
-        <v>0</v>
-      </c>
-      <c r="E23" s="52">
+      <c r="B23" s="33">
+        <v>0</v>
+      </c>
+      <c r="C23" s="41">
+        <v>0</v>
+      </c>
+      <c r="D23" s="41">
+        <v>0</v>
+      </c>
+      <c r="E23" s="50">
         <f>D16</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="F23" s="52">
+      <c r="F23" s="50">
         <f>D16</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="G23" s="52">
+      <c r="G23" s="50">
         <f>D14</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="H23" s="43">
-        <v>0</v>
-      </c>
-      <c r="I23" s="44">
+      <c r="H23" s="41">
+        <v>0</v>
+      </c>
+      <c r="I23" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="35">
-        <v>0</v>
-      </c>
-      <c r="C24" s="43">
-        <v>0</v>
-      </c>
-      <c r="D24" s="43">
-        <v>0</v>
-      </c>
-      <c r="E24" s="43">
-        <v>0</v>
-      </c>
-      <c r="F24" s="52">
-        <v>0</v>
-      </c>
-      <c r="G24" s="52">
+      <c r="B24" s="33">
+        <v>0</v>
+      </c>
+      <c r="C24" s="41">
+        <v>0</v>
+      </c>
+      <c r="D24" s="41">
+        <v>0</v>
+      </c>
+      <c r="E24" s="41">
+        <v>0</v>
+      </c>
+      <c r="F24" s="50">
+        <v>0</v>
+      </c>
+      <c r="G24" s="50">
         <f>D16</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="H24" s="43">
-        <v>0</v>
-      </c>
-      <c r="I24" s="44">
+      <c r="H24" s="41">
+        <v>0</v>
+      </c>
+      <c r="I24" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="35">
-        <v>0</v>
-      </c>
-      <c r="C25" s="43">
-        <v>0</v>
-      </c>
-      <c r="D25" s="43">
-        <v>0</v>
-      </c>
-      <c r="E25" s="43">
-        <v>0</v>
-      </c>
-      <c r="F25" s="43">
-        <v>0</v>
-      </c>
-      <c r="G25" s="52">
+      <c r="B25" s="33">
+        <v>0</v>
+      </c>
+      <c r="C25" s="41">
+        <v>0</v>
+      </c>
+      <c r="D25" s="41">
+        <v>0</v>
+      </c>
+      <c r="E25" s="41">
+        <v>0</v>
+      </c>
+      <c r="F25" s="41">
+        <v>0</v>
+      </c>
+      <c r="G25" s="50">
         <f>D15</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="H25" s="43">
-        <v>0</v>
-      </c>
-      <c r="I25" s="53">
+      <c r="H25" s="41">
+        <v>0</v>
+      </c>
+      <c r="I25" s="51">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="35">
-        <v>0</v>
-      </c>
-      <c r="C26" s="52">
-        <v>0</v>
-      </c>
-      <c r="D26" s="43">
-        <v>0</v>
-      </c>
-      <c r="E26" s="43">
-        <v>0</v>
-      </c>
-      <c r="F26" s="43">
-        <v>0</v>
-      </c>
-      <c r="G26" s="43">
-        <v>0</v>
-      </c>
-      <c r="H26" s="43">
-        <v>0</v>
-      </c>
-      <c r="I26" s="53">
+      <c r="B26" s="33">
+        <v>0</v>
+      </c>
+      <c r="C26" s="50">
+        <v>0</v>
+      </c>
+      <c r="D26" s="41">
+        <v>0</v>
+      </c>
+      <c r="E26" s="41">
+        <v>0</v>
+      </c>
+      <c r="F26" s="41">
+        <v>0</v>
+      </c>
+      <c r="G26" s="41">
+        <v>0</v>
+      </c>
+      <c r="H26" s="41">
+        <v>0</v>
+      </c>
+      <c r="I26" s="51">
         <f>D16</f>
         <v>1503.9206970584871</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="54">
-        <v>0</v>
-      </c>
-      <c r="C27" s="52">
+      <c r="B27" s="52">
+        <v>0</v>
+      </c>
+      <c r="C27" s="50">
         <f>D13</f>
         <v>4562.1665434388442</v>
       </c>
-      <c r="D27" s="52">
+      <c r="D27" s="50">
         <f>D16</f>
         <v>1503.9206970584871</v>
       </c>
-      <c r="E27" s="52">
-        <v>0</v>
-      </c>
-      <c r="F27" s="43">
-        <v>0</v>
-      </c>
-      <c r="G27" s="52">
-        <v>0</v>
-      </c>
-      <c r="H27" s="43">
-        <v>0</v>
-      </c>
-      <c r="I27" s="44">
+      <c r="E27" s="50">
+        <v>0</v>
+      </c>
+      <c r="F27" s="41">
+        <v>0</v>
+      </c>
+      <c r="G27" s="50">
+        <v>0</v>
+      </c>
+      <c r="H27" s="41">
+        <v>0</v>
+      </c>
+      <c r="I27" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="36">
-        <v>0</v>
-      </c>
-      <c r="C28" s="45">
-        <v>0</v>
-      </c>
-      <c r="D28" s="45">
-        <v>0</v>
-      </c>
-      <c r="E28" s="45">
-        <v>0</v>
-      </c>
-      <c r="F28" s="45">
-        <v>0</v>
-      </c>
-      <c r="G28" s="45">
-        <v>0</v>
-      </c>
-      <c r="H28" s="45">
-        <v>0</v>
-      </c>
-      <c r="I28" s="46">
+      <c r="B28" s="34">
+        <v>0</v>
+      </c>
+      <c r="C28" s="43">
+        <v>0</v>
+      </c>
+      <c r="D28" s="43">
+        <v>0</v>
+      </c>
+      <c r="E28" s="43">
+        <v>0</v>
+      </c>
+      <c r="F28" s="43">
+        <v>0</v>
+      </c>
+      <c r="G28" s="43">
+        <v>0</v>
+      </c>
+      <c r="H28" s="43">
+        <v>0</v>
+      </c>
+      <c r="I28" s="44">
         <v>0</v>
       </c>
     </row>

</xml_diff>